<commit_message>
Changes to the excel to accomodate new values
</commit_message>
<xml_diff>
--- a/sim/knn_datasets.xlsx
+++ b/sim/knn_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Documents/[DOCUMENTS].academic/[2018-now].inesc-id/KNNSimulator/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C28B77-AD75-7646-83E4-32EBBC6C1B8A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDF1266-2FC0-6948-B376-F4346B128E2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="0" windowWidth="23200" windowHeight="21000" activeTab="4" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>Poker Hand</t>
   </si>
@@ -196,6 +196,27 @@
   </si>
   <si>
     <t>Intel(R) Xeon(R) CPU E5450 @ 3.00GHz (x2)</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Associativity</t>
+  </si>
+  <si>
+    <t>Separate data/instruction</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Harpertown</t>
   </si>
 </sst>
 </file>
@@ -276,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -548,6 +569,48 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -558,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,14 +716,44 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1000,7 +1093,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1215,269 +1308,315 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC5BBDF-4529-454A-B47D-B01993F61E5D}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="42" customFormat="1">
+    <row r="1" spans="1:13" s="42" customFormat="1">
       <c r="A1" s="33"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
+    </row>
+    <row r="2" spans="1:13" s="42" customFormat="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" s="37" customFormat="1" ht="17" thickBot="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="M2" s="62"/>
+    </row>
+    <row r="3" spans="1:13" s="50" customFormat="1" ht="17" thickBot="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D3" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="G3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="H3" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="M3" s="51" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="34" customFormat="1">
-      <c r="A3" s="33" t="s">
+    <row r="4" spans="1:13" s="34" customFormat="1">
+      <c r="A4" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B4" s="58">
         <v>3.9</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C4" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="34">
+      <c r="E4" s="34">
         <v>0.7</v>
       </c>
-      <c r="E3" s="34">
+      <c r="F4" s="34">
         <v>1</v>
       </c>
-      <c r="F3" s="40">
+      <c r="G4" s="40">
         <v>1</v>
       </c>
-      <c r="G3" s="34">
+      <c r="L4" s="58">
         <v>0.5</v>
       </c>
-      <c r="H3" s="40"/>
-    </row>
-    <row r="4" spans="1:8" s="15" customFormat="1">
-      <c r="A4" s="3" t="s">
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="1:13" s="15" customFormat="1">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B5" s="14">
         <v>5.7</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="15">
+      <c r="E5" s="15">
         <v>1.6</v>
       </c>
-      <c r="E4" s="15">
+      <c r="F5" s="15">
         <v>4</v>
       </c>
-      <c r="F4" s="16">
+      <c r="G5" s="16">
         <v>4</v>
       </c>
-      <c r="G4" s="19">
+      <c r="L5" s="59">
         <v>2</v>
       </c>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" s="36" customFormat="1" ht="17" thickBot="1">
-      <c r="A5" s="35" t="s">
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="1:13" s="36" customFormat="1" ht="17" thickBot="1">
+      <c r="A6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B6" s="60">
         <v>4.7</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C6" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="36">
+      <c r="E6" s="36">
         <v>1.4</v>
       </c>
-      <c r="E5" s="36">
+      <c r="F6" s="36">
         <v>4</v>
       </c>
-      <c r="F5" s="41">
+      <c r="G6" s="41">
         <v>4</v>
       </c>
-      <c r="G5" s="36">
+      <c r="L6" s="60">
         <v>1</v>
       </c>
-      <c r="H5" s="41">
+      <c r="M6" s="41">
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B7" s="59">
         <v>145</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="19">
+      <c r="E7" s="19">
         <v>2.4</v>
       </c>
-      <c r="E6" s="19">
+      <c r="F7" s="19">
         <v>4</v>
       </c>
-      <c r="F6" s="16">
+      <c r="G7" s="16">
         <v>4</v>
       </c>
-      <c r="G6" s="19">
+      <c r="L7" s="59">
         <v>4</v>
       </c>
-      <c r="H6" s="16">
+      <c r="M7" s="16">
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B8" s="59">
         <v>62</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="15">
+      <c r="E8" s="15">
         <v>2.9</v>
       </c>
-      <c r="E7" s="15">
+      <c r="F8" s="15">
         <v>4</v>
       </c>
-      <c r="F7" s="16">
+      <c r="G8" s="16">
         <v>8</v>
       </c>
-      <c r="G7" s="19">
+      <c r="L8" s="59">
         <v>16</v>
       </c>
-      <c r="H7" s="16">
+      <c r="M8" s="16">
         <v>2133</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:13">
+      <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B9" s="14">
         <v>75</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="19">
+      <c r="E9" s="19">
         <v>3.5</v>
       </c>
-      <c r="E8" s="19">
+      <c r="F9" s="19">
         <v>2</v>
       </c>
-      <c r="F8" s="16">
+      <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="L9" s="59">
         <v>8</v>
       </c>
-      <c r="H8" s="16">
+      <c r="M9" s="16">
         <v>1600</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B10" s="14">
         <v>135</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="19">
+      <c r="E10" s="19">
         <v>3</v>
       </c>
-      <c r="E9" s="19">
+      <c r="F10" s="19">
         <v>2</v>
       </c>
-      <c r="F9" s="16">
+      <c r="G10" s="16">
         <v>2</v>
       </c>
-      <c r="G9" s="19">
+      <c r="L10" s="59">
         <v>4</v>
       </c>
-      <c r="H9" s="16">
+      <c r="M10" s="16">
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B11" s="14">
         <v>347</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D11" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="19">
         <v>3</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F11" s="19">
         <v>8</v>
       </c>
-      <c r="F10" s="16">
+      <c r="G11" s="16">
         <v>8</v>
       </c>
-      <c r="G10" s="19">
+      <c r="L11" s="59">
         <v>32</v>
       </c>
-      <c r="H10" s="16">
+      <c r="M11" s="16">
         <v>667</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C1:F1"/>
+  <mergeCells count="4">
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1488,7 +1627,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1993,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40F9C77-6425-6D4E-BBF1-9B74B3972FC3}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Excel modifications; created power analysis script
</commit_message>
<xml_diff>
--- a/sim/knn_datasets.xlsx
+++ b/sim/knn_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Documents/[DOCUMENTS].academic/[2018-now].inesc-id/KNNSimulator/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BE541F-2AD0-9648-9879-4E5210FD8F64}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92C17FA-4314-C948-9E48-83B681E9759D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="1" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -699,43 +699,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,15 +711,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD241F55-EC18-3E4B-8A05-E2467D6A30F5}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1311,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC5BBDF-4529-454A-B47D-B01993F61E5D}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1333,75 +1333,75 @@
   <sheetData>
     <row r="1" spans="1:13" s="42" customFormat="1">
       <c r="A1" s="33"/>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="56"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="64"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="51"/>
     </row>
     <row r="2" spans="1:13" s="42" customFormat="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50" t="s">
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="53" t="s">
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="62"/>
-    </row>
-    <row r="3" spans="1:13" s="50" customFormat="1" ht="17" thickBot="1">
+      <c r="M2" s="53"/>
+    </row>
+    <row r="3" spans="1:13" s="44" customFormat="1" ht="17" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="57" t="s">
+      <c r="L3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="51" t="s">
+      <c r="M3" s="45" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1409,10 +1409,10 @@
       <c r="A4" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="47">
         <v>3.9</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="47" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="34">
@@ -1424,7 +1424,7 @@
       <c r="G4" s="40">
         <v>1</v>
       </c>
-      <c r="L4" s="58">
+      <c r="L4" s="47">
         <v>0.5</v>
       </c>
       <c r="M4" s="40"/>
@@ -1448,7 +1448,7 @@
       <c r="G5" s="16">
         <v>4</v>
       </c>
-      <c r="L5" s="59">
+      <c r="L5" s="48">
         <v>2</v>
       </c>
       <c r="M5" s="16"/>
@@ -1457,10 +1457,10 @@
       <c r="A6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="49">
         <v>4.7</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="49" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="36">
@@ -1472,7 +1472,7 @@
       <c r="G6" s="41">
         <v>4</v>
       </c>
-      <c r="L6" s="60">
+      <c r="L6" s="49">
         <v>1</v>
       </c>
       <c r="M6" s="41">
@@ -1483,7 +1483,7 @@
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="48">
         <v>145</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -1498,7 +1498,7 @@
       <c r="G7" s="16">
         <v>4</v>
       </c>
-      <c r="L7" s="59">
+      <c r="L7" s="48">
         <v>4</v>
       </c>
       <c r="M7" s="16">
@@ -1509,7 +1509,7 @@
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="48">
         <v>62</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1524,7 +1524,7 @@
       <c r="G8" s="16">
         <v>8</v>
       </c>
-      <c r="L8" s="59">
+      <c r="L8" s="48">
         <v>16</v>
       </c>
       <c r="M8" s="16">
@@ -1550,7 +1550,7 @@
       <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="L9" s="59">
+      <c r="L9" s="48">
         <v>8</v>
       </c>
       <c r="M9" s="16">
@@ -1576,7 +1576,7 @@
       <c r="G10" s="16">
         <v>2</v>
       </c>
-      <c r="L10" s="59">
+      <c r="L10" s="48">
         <v>4</v>
       </c>
       <c r="M10" s="16">
@@ -1605,7 +1605,7 @@
       <c r="G11" s="16">
         <v>8</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L11" s="48">
         <v>32</v>
       </c>
       <c r="M11" s="16">
@@ -1809,14 +1809,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" s="21" customFormat="1">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2109,17 +2109,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="20" customFormat="1">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2163,18 +2163,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="42" customFormat="1">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="44" t="s">
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="45"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:9" s="43" customFormat="1" ht="17" thickBot="1">
       <c r="A2" s="38"/>

</xml_diff>

<commit_message>
Added timing results for 24 accelerators on ZedBoard
</commit_message>
<xml_diff>
--- a/sim/knn_datasets.xlsx
+++ b/sim/knn_datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Documents/[DOCUMENTS].academic/[2018-now].inesc-id/KNNSimulator/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92C17FA-4314-C948-9E48-83B681E9759D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636A17C1-3F26-7A44-A853-5DE207E39446}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="1" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" activeTab="5" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -760,7 +761,67 @@
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1094,7 +1155,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1289,7 +1350,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{3DE48AAC-DC80-B744-9C46-F3A37EEF6D7A}">
-    <sortState ref="A2:F9">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
       <sortCondition ref="B1:B9"/>
     </sortState>
   </autoFilter>
@@ -1311,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC5BBDF-4529-454A-B47D-B01993F61E5D}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1625,20 +1686,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CB9E5A-F363-4F4F-9FB0-1E4522628289}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.5" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="17" thickBot="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1657,8 +1718,11 @@
       <c r="F1" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1677,8 +1741,11 @@
       <c r="F2" s="13">
         <v>263.83</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>293.08999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1697,8 +1764,11 @@
       <c r="F3" s="13">
         <v>315.04000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>332.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1717,8 +1787,11 @@
       <c r="F4" s="13">
         <v>2130.86</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>1677.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1737,8 +1810,11 @@
       <c r="F5" s="13">
         <v>4854.58</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>4014.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1757,8 +1833,11 @@
       <c r="F6" s="13">
         <v>27328.47</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="30" customFormat="1">
+      <c r="G6">
+        <v>20894.650000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="30" customFormat="1">
       <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
@@ -1768,7 +1847,7 @@
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1787,8 +1866,11 @@
       <c r="F8" s="13">
         <v>4608785.8600000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>3092637.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1807,8 +1889,11 @@
       <c r="F9" s="13">
         <v>161057301.38</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="21" customFormat="1">
+      <c r="G9" s="13">
+        <v>108882432.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="21" customFormat="1">
       <c r="A10" s="60" t="s">
         <v>34</v>
       </c>
@@ -2145,8 +2230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40F9C77-6425-6D4E-BBF1-9B74B3972FC3}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2220,24 +2305,24 @@
         <v>4.4270932039570932</v>
       </c>
       <c r="E3" s="23">
-        <f>'Timing CPU'!E2/'Timing Accel'!$F2*1000000</f>
-        <v>3.7562066482204446</v>
+        <f>'Timing CPU'!E2/'Timing Accel'!$G2*1000000</f>
+        <v>3.3812139615817669</v>
       </c>
       <c r="F3" s="24">
-        <f>'Timing CPU'!F2/'Timing Accel'!$F2*1000000</f>
-        <v>0.7618542243111095</v>
+        <f>'Timing CPU'!F2/'Timing Accel'!$G2*1000000</f>
+        <v>0.68579617182435437</v>
       </c>
       <c r="G3" s="24">
-        <f>'Timing CPU'!G2/'Timing Accel'!$F2*1000000</f>
-        <v>0.82249933669408337</v>
+        <f>'Timing CPU'!G2/'Timing Accel'!$G2*1000000</f>
+        <v>0.74038691187007399</v>
       </c>
       <c r="H3" s="24">
-        <f>'Timing CPU'!H2/'Timing Accel'!$F2*1000000</f>
-        <v>1.8079824129174089</v>
+        <f>'Timing CPU'!H2/'Timing Accel'!$G2*1000000</f>
+        <v>1.62748643761302</v>
       </c>
       <c r="I3" s="25">
-        <f>'Timing CPU'!I2/'Timing Accel'!$F2*1000000</f>
-        <v>2.020240306257818</v>
+        <f>'Timing CPU'!I2/'Timing Accel'!$G2*1000000</f>
+        <v>1.8185540277730394</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2257,24 +2342,24 @@
         <v>4.9771457592686632</v>
       </c>
       <c r="E4" s="23">
-        <f>'Timing CPU'!E3/'Timing Accel'!$F3*1000000</f>
-        <v>3.297993905535805</v>
+        <f>'Timing CPU'!E3/'Timing Accel'!$G3*1000000</f>
+        <v>3.1244361580561733</v>
       </c>
       <c r="F4" s="24">
-        <f>'Timing CPU'!F3/'Timing Accel'!$F3*1000000</f>
-        <v>0.6094464195022854</v>
+        <f>'Timing CPU'!F3/'Timing Accel'!$G3*1000000</f>
+        <v>0.57737415047813789</v>
       </c>
       <c r="G4" s="24">
-        <f>'Timing CPU'!G3/'Timing Accel'!$F3*1000000</f>
-        <v>1.2252412392077194</v>
+        <f>'Timing CPU'!G3/'Timing Accel'!$G3*1000000</f>
+        <v>1.1607626150237564</v>
       </c>
       <c r="H4" s="24">
-        <f>'Timing CPU'!H3/'Timing Accel'!$F3*1000000</f>
-        <v>2.7837734890807511</v>
+        <f>'Timing CPU'!H3/'Timing Accel'!$G3*1000000</f>
+        <v>2.6372767185902446</v>
       </c>
       <c r="I4" s="25">
-        <f>'Timing CPU'!I3/'Timing Accel'!$F3*1000000</f>
-        <v>1.8315134586084305</v>
+        <f>'Timing CPU'!I3/'Timing Accel'!$G3*1000000</f>
+        <v>1.7351296084681542</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2294,24 +2379,24 @@
         <v>5.1035732051847607</v>
       </c>
       <c r="E5" s="23">
-        <f>'Timing CPU'!E4/'Timing Accel'!$F4*1000000</f>
-        <v>0.92920229390950126</v>
+        <f>'Timing CPU'!E4/'Timing Accel'!$G4*1000000</f>
+        <v>1.1806093852483455</v>
       </c>
       <c r="F5" s="24">
-        <f>'Timing CPU'!F4/'Timing Accel'!$F4*1000000</f>
-        <v>0.32522080286832544</v>
+        <f>'Timing CPU'!F4/'Timing Accel'!$G4*1000000</f>
+        <v>0.41321328483692094</v>
       </c>
       <c r="G5" s="24">
-        <f>'Timing CPU'!G4/'Timing Accel'!$F4*1000000</f>
-        <v>1.2056165116431863</v>
+        <f>'Timing CPU'!G4/'Timing Accel'!$G4*1000000</f>
+        <v>1.5318108639914139</v>
       </c>
       <c r="H5" s="24">
-        <f>'Timing CPU'!H4/'Timing Accel'!$F4*1000000</f>
-        <v>5.9159212712238247</v>
+        <f>'Timing CPU'!H4/'Timing Accel'!$G4*1000000</f>
+        <v>7.5165464194144649</v>
       </c>
       <c r="I5" s="25">
-        <f>'Timing CPU'!I4/'Timing Accel'!$F4*1000000</f>
-        <v>0.85270735759270899</v>
+        <f>'Timing CPU'!I4/'Timing Accel'!$G4*1000000</f>
+        <v>1.0834178045435574</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2331,24 +2416,24 @@
         <v>6.83086899381615</v>
       </c>
       <c r="E6" s="23">
-        <f>'Timing CPU'!E5/'Timing Accel'!$F5*1000000</f>
-        <v>1.0272773339815184</v>
+        <f>'Timing CPU'!E5/'Timing Accel'!$G5*1000000</f>
+        <v>1.2421199977085415</v>
       </c>
       <c r="F6" s="24">
-        <f>'Timing CPU'!F5/'Timing Accel'!$F5*1000000</f>
-        <v>0.32196400100523626</v>
+        <f>'Timing CPU'!F5/'Timing Accel'!$G5*1000000</f>
+        <v>0.38929888839351318</v>
       </c>
       <c r="G6" s="24">
-        <f>'Timing CPU'!G5/'Timing Accel'!$F5*1000000</f>
-        <v>2.3528296989646891</v>
+        <f>'Timing CPU'!G5/'Timing Accel'!$G5*1000000</f>
+        <v>2.8448956514591859</v>
       </c>
       <c r="H6" s="24">
-        <f>'Timing CPU'!H5/'Timing Accel'!$F5*1000000</f>
-        <v>7.9040823305002705</v>
+        <f>'Timing CPU'!H5/'Timing Accel'!$G5*1000000</f>
+        <v>9.5571258135300674</v>
       </c>
       <c r="I6" s="25">
-        <f>'Timing CPU'!I5/'Timing Accel'!$F5*1000000</f>
-        <v>1.2421259923618519</v>
+        <f>'Timing CPU'!I5/'Timing Accel'!$G5*1000000</f>
+        <v>1.5019016615565481</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2368,24 +2453,24 @@
         <v>6.5872330210948515</v>
       </c>
       <c r="E7" s="23">
-        <f>'Timing CPU'!E6/'Timing Accel'!$F6*1000000</f>
-        <v>0.96459845721330162</v>
+        <f>'Timing CPU'!E6/'Timing Accel'!$G6*1000000</f>
+        <v>1.2616148152756803</v>
       </c>
       <c r="F7" s="24">
-        <f>'Timing CPU'!F6/'Timing Accel'!$F6*1000000</f>
-        <v>0.20528042733457089</v>
+        <f>'Timing CPU'!F6/'Timing Accel'!$G6*1000000</f>
+        <v>0.26848978087692305</v>
       </c>
       <c r="G7" s="24">
-        <f>'Timing CPU'!G6/'Timing Accel'!$F6*1000000</f>
-        <v>2.041204648485627</v>
+        <f>'Timing CPU'!G6/'Timing Accel'!$G6*1000000</f>
+        <v>2.6697264610797502</v>
       </c>
       <c r="H7" s="24">
-        <f>'Timing CPU'!H6/'Timing Accel'!$F6*1000000</f>
-        <v>9.5451007685391822</v>
+        <f>'Timing CPU'!H6/'Timing Accel'!$G6*1000000</f>
+        <v>12.484200501085205</v>
       </c>
       <c r="I7" s="25">
-        <f>'Timing CPU'!I6/'Timing Accel'!$F6*1000000</f>
-        <v>0.76846599901128743</v>
+        <f>'Timing CPU'!I6/'Timing Accel'!$G6*1000000</f>
+        <v>1.0050898196428271</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="30" customFormat="1">
@@ -2418,24 +2503,24 @@
         <v>8.9511446730571258</v>
       </c>
       <c r="E9" s="23">
-        <f>'Timing CPU'!E8/'Timing Accel'!$F8*1000000</f>
-        <v>0.8871629370951073</v>
+        <f>'Timing CPU'!E8/'Timing Accel'!$G8*1000000</f>
+        <v>1.3220897899386612</v>
       </c>
       <c r="F9" s="24">
-        <f>'Timing CPU'!F8/'Timing Accel'!$F8*1000000</f>
-        <v>0.2632389607270666</v>
+        <f>'Timing CPU'!F8/'Timing Accel'!$G8*1000000</f>
+        <v>0.39229044377223493</v>
       </c>
       <c r="G9" s="24">
-        <f>'Timing CPU'!G8/'Timing Accel'!$F8*1000000</f>
-        <v>0.8722357953077039</v>
+        <f>'Timing CPU'!G8/'Timing Accel'!$G8*1000000</f>
+        <v>1.2998446972675086</v>
       </c>
       <c r="H9" s="24">
-        <f>'Timing CPU'!H8/'Timing Accel'!$F8*1000000</f>
-        <v>10.347029445191016</v>
+        <f>'Timing CPU'!H8/'Timing Accel'!$G8*1000000</f>
+        <v>15.419604915500676</v>
       </c>
       <c r="I9" s="25">
-        <f>'Timing CPU'!I8/'Timing Accel'!$F8*1000000</f>
-        <v>0.36220841035126761</v>
+        <f>'Timing CPU'!I8/'Timing Accel'!$G8*1000000</f>
+        <v>0.53977913315824977</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2455,24 +2540,24 @@
         <v>9.7685731197491155</v>
       </c>
       <c r="E10" s="23">
-        <f>'Timing CPU'!E9/'Timing Accel'!$F9*1000000</f>
-        <v>1.4490380255991349</v>
+        <f>'Timing CPU'!E9/'Timing Accel'!$G9*1000000</f>
+        <v>2.1433958444763919</v>
       </c>
       <c r="F10" s="24">
-        <f>'Timing CPU'!F9/'Timing Accel'!$F9*1000000</f>
-        <v>0.34632865770174004</v>
+        <f>'Timing CPU'!F9/'Timing Accel'!$G9*1000000</f>
+        <v>0.51228428283244609</v>
       </c>
       <c r="G10" s="24">
-        <f>'Timing CPU'!G9/'Timing Accel'!$F9*1000000</f>
-        <v>1.0662947940174907</v>
+        <f>'Timing CPU'!G9/'Timing Accel'!$G9*1000000</f>
+        <v>1.57724765679556</v>
       </c>
       <c r="H10" s="24">
-        <f>'Timing CPU'!H9/'Timing Accel'!$F9*1000000</f>
-        <v>11.977896111945894</v>
+        <f>'Timing CPU'!H9/'Timing Accel'!$G9*1000000</f>
+        <v>17.717528662713718</v>
       </c>
       <c r="I10" s="25">
-        <f>'Timing CPU'!I9/'Timing Accel'!$F9*1000000</f>
-        <v>0.58399147504702831</v>
+        <f>'Timing CPU'!I9/'Timing Accel'!$G9*1000000</f>
+        <v>0.86383164465810869</v>
       </c>
     </row>
   </sheetData>
@@ -2481,10 +2566,10 @@
     <mergeCell ref="E1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:I7 B9:I10">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Corrected power analysis script and processed power consumption logs of Intel based machines
</commit_message>
<xml_diff>
--- a/sim/knn_datasets.xlsx
+++ b/sim/knn_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Documents/[DOCUMENTS].academic/[2018-now].inesc-id/KNNSimulator/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636A17C1-3F26-7A44-A853-5DE207E39446}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECEB9D1-A42F-4E45-A9B5-FB62AF99BF99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" activeTab="5" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
   <si>
     <t>Poker Hand</t>
   </si>
@@ -219,6 +219,27 @@
   </si>
   <si>
     <t>Harpertown</t>
+  </si>
+  <si>
+    <t>Values in watts</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Idle</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
   </si>
 </sst>
 </file>
@@ -299,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -610,6 +631,39 @@
     <border>
       <left/>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -623,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -756,72 +810,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1155,7 +1176,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1373,7 +1394,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1916,7 +1937,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2216,12 +2237,250 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93596D3-9253-B144-BE5D-2C514E5B9E89}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A1" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="77">
+        <v>79</v>
+      </c>
+      <c r="G2" s="77">
+        <v>15</v>
+      </c>
+      <c r="H2" s="77">
+        <v>45</v>
+      </c>
+      <c r="I2" s="77">
+        <v>74</v>
+      </c>
+      <c r="J2" s="13">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="70"/>
+      <c r="B3" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="13">
+        <v>95</v>
+      </c>
+      <c r="G3" s="13">
+        <v>20</v>
+      </c>
+      <c r="H3" s="13">
+        <v>52</v>
+      </c>
+      <c r="I3" s="13">
+        <v>83</v>
+      </c>
+      <c r="J3" s="13">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="70"/>
+      <c r="B4" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="13">
+        <v>83.400249876800004</v>
+      </c>
+      <c r="G4" s="13">
+        <v>17.063609822899998</v>
+      </c>
+      <c r="H4" s="13">
+        <v>48.795460974400001</v>
+      </c>
+      <c r="I4" s="13">
+        <v>78.114444090500001</v>
+      </c>
+      <c r="J4" s="13">
+        <v>233.106558621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="75" customFormat="1">
+      <c r="A5" s="72"/>
+      <c r="B5" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="74"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="78">
+        <v>2.5453206508499999</v>
+      </c>
+      <c r="G5" s="78">
+        <v>1.03317437585</v>
+      </c>
+      <c r="H5" s="78">
+        <v>1.1970549137399999</v>
+      </c>
+      <c r="I5" s="78">
+        <v>1.9350476632</v>
+      </c>
+      <c r="J5" s="78">
+        <v>4.1344574757599997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="13">
+        <v>82</v>
+      </c>
+      <c r="G6" s="13">
+        <v>16</v>
+      </c>
+      <c r="H6" s="13">
+        <v>48</v>
+      </c>
+      <c r="I6" s="13">
+        <v>74</v>
+      </c>
+      <c r="J6" s="13">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="70"/>
+      <c r="B7" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="13">
+        <v>161</v>
+      </c>
+      <c r="G7" s="13">
+        <v>66</v>
+      </c>
+      <c r="H7" s="13">
+        <v>79</v>
+      </c>
+      <c r="I7" s="79">
+        <v>149</v>
+      </c>
+      <c r="J7" s="80">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="70"/>
+      <c r="B8" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="13">
+        <v>150.733263029</v>
+      </c>
+      <c r="G8" s="13">
+        <v>55.030479873300003</v>
+      </c>
+      <c r="H8" s="13">
+        <v>74.802833365300003</v>
+      </c>
+      <c r="I8" s="13">
+        <v>141.69338719699999</v>
+      </c>
+      <c r="J8" s="13">
+        <v>330.97444960000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="70"/>
+      <c r="B9" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="13">
+        <v>0.10434324846</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0.14542360448300001</v>
+      </c>
+      <c r="H9" s="13">
+        <v>8.3724022653700006E-2</v>
+      </c>
+      <c r="I9" s="13">
+        <v>3.1785635094099998E-2</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0.21005931907200001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="20" customFormat="1">
+      <c r="A10" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2230,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40F9C77-6425-6D4E-BBF1-9B74B3972FC3}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2566,10 +2825,10 @@
     <mergeCell ref="E1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:I7 B9:I10">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated power results on excel
</commit_message>
<xml_diff>
--- a/sim/knn_datasets.xlsx
+++ b/sim/knn_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Documents/[DOCUMENTS].academic/[2018-now].inesc-id/KNNSimulator/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECEB9D1-A42F-4E45-A9B5-FB62AF99BF99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A9622C-2149-F44A-8552-FDD611D279B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" activeTab="1" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -768,64 +768,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -837,6 +786,57 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1391,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC5BBDF-4529-454A-B47D-B01993F61E5D}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1408,54 +1408,51 @@
     <col min="8" max="8" width="22.5" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="13" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="42" customFormat="1">
+    <row r="1" spans="1:12" s="42" customFormat="1">
       <c r="A1" s="33"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="56"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44" t="s">
         <v>53</v>
       </c>
       <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51"/>
-    </row>
-    <row r="2" spans="1:13" s="42" customFormat="1">
+      <c r="K1" s="50"/>
+      <c r="L1" s="51"/>
+    </row>
+    <row r="2" spans="1:12" s="42" customFormat="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="52" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="53"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="65"/>
       <c r="H2" s="44"/>
       <c r="I2" s="44" t="s">
         <v>54</v>
       </c>
       <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="52" t="s">
+      <c r="K2" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="53"/>
-    </row>
-    <row r="3" spans="1:13" s="44" customFormat="1" ht="17" thickBot="1">
+      <c r="L2" s="65"/>
+    </row>
+    <row r="3" spans="1:12" s="44" customFormat="1" ht="17" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="58"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="46" t="s">
         <v>37</v>
       </c>
@@ -1480,14 +1477,14 @@
       <c r="J3" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="K3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="L3" s="45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="34" customFormat="1">
+    <row r="4" spans="1:12" s="34" customFormat="1">
       <c r="A4" s="33" t="s">
         <v>25</v>
       </c>
@@ -1506,12 +1503,12 @@
       <c r="G4" s="40">
         <v>1</v>
       </c>
-      <c r="L4" s="47">
+      <c r="K4" s="47">
         <v>0.5</v>
       </c>
-      <c r="M4" s="40"/>
-    </row>
-    <row r="5" spans="1:13" s="15" customFormat="1">
+      <c r="L4" s="40"/>
+    </row>
+    <row r="5" spans="1:12" s="15" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1530,12 +1527,12 @@
       <c r="G5" s="16">
         <v>4</v>
       </c>
-      <c r="L5" s="48">
+      <c r="K5" s="48">
         <v>2</v>
       </c>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:13" s="36" customFormat="1" ht="17" thickBot="1">
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6" spans="1:12" s="36" customFormat="1" ht="17" thickBot="1">
       <c r="A6" s="35" t="s">
         <v>27</v>
       </c>
@@ -1554,14 +1551,14 @@
       <c r="G6" s="41">
         <v>4</v>
       </c>
-      <c r="L6" s="49">
+      <c r="K6" s="49">
         <v>1</v>
       </c>
-      <c r="M6" s="41">
+      <c r="L6" s="41">
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1580,14 +1577,14 @@
       <c r="G7" s="16">
         <v>4</v>
       </c>
-      <c r="L7" s="48">
+      <c r="K7" s="48">
         <v>4</v>
       </c>
-      <c r="M7" s="16">
+      <c r="L7" s="16">
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -1606,14 +1603,14 @@
       <c r="G8" s="16">
         <v>8</v>
       </c>
-      <c r="L8" s="48">
+      <c r="K8" s="48">
         <v>16</v>
       </c>
-      <c r="M8" s="16">
+      <c r="L8" s="16">
         <v>2133</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1632,14 +1629,14 @@
       <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="L9" s="48">
+      <c r="K9" s="48">
         <v>8</v>
       </c>
-      <c r="M9" s="16">
+      <c r="L9" s="16">
         <v>1600</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1658,14 +1655,14 @@
       <c r="G10" s="16">
         <v>2</v>
       </c>
-      <c r="L10" s="48">
+      <c r="K10" s="48">
         <v>4</v>
       </c>
-      <c r="M10" s="16">
+      <c r="L10" s="16">
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1687,16 +1684,16 @@
       <c r="G11" s="16">
         <v>8</v>
       </c>
-      <c r="L11" s="48">
+      <c r="K11" s="48">
         <v>32</v>
       </c>
-      <c r="M11" s="16">
+      <c r="L11" s="16">
         <v>667</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C2:G2"/>
@@ -1915,14 +1912,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="21" customFormat="1">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1937,7 +1934,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2215,17 +2212,17 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="20" customFormat="1">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2239,14 +2236,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93596D3-9253-B144-BE5D-2C514E5B9E89}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="5" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="67" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
@@ -2257,10 +2254,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="17" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="17" t="s">
         <v>25</v>
       </c>
@@ -2287,22 +2284,22 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="77">
+      <c r="F2" s="60">
         <v>79</v>
       </c>
-      <c r="G2" s="77">
+      <c r="G2" s="60">
         <v>15</v>
       </c>
-      <c r="H2" s="77">
+      <c r="H2" s="60">
         <v>45</v>
       </c>
-      <c r="I2" s="77">
+      <c r="I2" s="60">
         <v>74</v>
       </c>
       <c r="J2" s="13">
@@ -2310,8 +2307,8 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="70"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="76"/>
+      <c r="B3" s="52" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="13">
@@ -2331,8 +2328,8 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="70"/>
-      <c r="B4" s="66" t="s">
+      <c r="A4" s="76"/>
+      <c r="B4" s="52" t="s">
         <v>63</v>
       </c>
       <c r="F4" s="13">
@@ -2351,34 +2348,34 @@
         <v>233.106558621</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="75" customFormat="1">
-      <c r="A5" s="72"/>
-      <c r="B5" s="73" t="s">
+    <row r="5" spans="1:10" s="58" customFormat="1">
+      <c r="A5" s="77"/>
+      <c r="B5" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="78">
+      <c r="C5" s="57"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="61">
         <v>2.5453206508499999</v>
       </c>
-      <c r="G5" s="78">
+      <c r="G5" s="61">
         <v>1.03317437585</v>
       </c>
-      <c r="H5" s="78">
+      <c r="H5" s="61">
         <v>1.1970549137399999</v>
       </c>
-      <c r="I5" s="78">
+      <c r="I5" s="61">
         <v>1.9350476632</v>
       </c>
-      <c r="J5" s="78">
+      <c r="J5" s="61">
         <v>4.1344574757599997</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="55" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="13">
@@ -2398,8 +2395,8 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="70"/>
-      <c r="B7" s="66" t="s">
+      <c r="A7" s="76"/>
+      <c r="B7" s="52" t="s">
         <v>62</v>
       </c>
       <c r="F7" s="13">
@@ -2411,16 +2408,16 @@
       <c r="H7" s="13">
         <v>79</v>
       </c>
-      <c r="I7" s="79">
+      <c r="I7" s="62">
         <v>149</v>
       </c>
-      <c r="J7" s="80">
+      <c r="J7" s="63">
         <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="70"/>
-      <c r="B8" s="66" t="s">
+      <c r="A8" s="76"/>
+      <c r="B8" s="52" t="s">
         <v>63</v>
       </c>
       <c r="F8" s="13">
@@ -2440,8 +2437,8 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="70"/>
-      <c r="B9" s="73" t="s">
+      <c r="A9" s="76"/>
+      <c r="B9" s="56" t="s">
         <v>66</v>
       </c>
       <c r="F9" s="13">
@@ -2461,18 +2458,18 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="20" customFormat="1">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2490,7 +2487,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2507,18 +2504,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="42" customFormat="1">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="63" t="s">
+      <c r="C1" s="79"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="65"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="80"/>
     </row>
     <row r="2" spans="1:9" s="43" customFormat="1" ht="17" thickBot="1">
       <c r="A2" s="38"/>
@@ -2552,16 +2549,16 @@
         <v>16</v>
       </c>
       <c r="B3" s="23">
-        <f>'Timing CPU'!B2/'Timing Accel'!$F2*1000000</f>
-        <v>10.116362809384832</v>
+        <f>'Timing CPU'!B2/'Timing Accel'!$G2*1000000</f>
+        <v>9.106417823876626</v>
       </c>
       <c r="C3" s="24">
-        <f>'Timing CPU'!C2/'Timing Accel'!$F2*1000000</f>
-        <v>2.649433347231172</v>
+        <f>'Timing CPU'!C2/'Timing Accel'!$G2*1000000</f>
+        <v>2.3849329557473813</v>
       </c>
       <c r="D3" s="25">
-        <f>'Timing CPU'!D2/'Timing Accel'!$F2*1000000</f>
-        <v>4.4270932039570932</v>
+        <f>'Timing CPU'!D2/'Timing Accel'!$G2*1000000</f>
+        <v>3.9851240233375416</v>
       </c>
       <c r="E3" s="23">
         <f>'Timing CPU'!E2/'Timing Accel'!$G2*1000000</f>
@@ -2589,16 +2586,16 @@
         <v>14</v>
       </c>
       <c r="B4" s="23">
-        <f>'Timing CPU'!B3/'Timing Accel'!$F3*1000000</f>
-        <v>14.62671406805485</v>
+        <f>'Timing CPU'!B3/'Timing Accel'!$G3*1000000</f>
+        <v>13.85697961147531</v>
       </c>
       <c r="C4" s="24">
-        <f>'Timing CPU'!C3/'Timing Accel'!$F3*1000000</f>
-        <v>3.5170137125444385</v>
+        <f>'Timing CPU'!C3/'Timing Accel'!$G3*1000000</f>
+        <v>3.3319299933842546</v>
       </c>
       <c r="D4" s="25">
-        <f>'Timing CPU'!D3/'Timing Accel'!$F3*1000000</f>
-        <v>4.9771457592686632</v>
+        <f>'Timing CPU'!D3/'Timing Accel'!$G3*1000000</f>
+        <v>4.7152222289047927</v>
       </c>
       <c r="E4" s="23">
         <f>'Timing CPU'!E3/'Timing Accel'!$G3*1000000</f>
@@ -2626,16 +2623,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="23">
-        <f>'Timing CPU'!B4/'Timing Accel'!$F4*1000000</f>
-        <v>44.605933754446554</v>
+        <f>'Timing CPU'!B4/'Timing Accel'!$G4*1000000</f>
+        <v>56.67461689821716</v>
       </c>
       <c r="C5" s="24">
-        <f>'Timing CPU'!C4/'Timing Accel'!$F4*1000000</f>
-        <v>5.8253475122720406</v>
+        <f>'Timing CPU'!C4/'Timing Accel'!$G4*1000000</f>
+        <v>7.401466817721067</v>
       </c>
       <c r="D5" s="25">
-        <f>'Timing CPU'!D4/'Timing Accel'!$F4*1000000</f>
-        <v>5.1035732051847607</v>
+        <f>'Timing CPU'!D4/'Timing Accel'!$G4*1000000</f>
+        <v>6.484407608371594</v>
       </c>
       <c r="E5" s="23">
         <f>'Timing CPU'!E4/'Timing Accel'!$G4*1000000</f>
@@ -2663,16 +2660,16 @@
         <v>11</v>
       </c>
       <c r="B6" s="23">
-        <f>'Timing CPU'!B5/'Timing Accel'!$F5*1000000</f>
-        <v>58.457168282323089</v>
+        <f>'Timing CPU'!B5/'Timing Accel'!$G5*1000000</f>
+        <v>70.682779937781916</v>
       </c>
       <c r="C6" s="24">
-        <f>'Timing CPU'!C5/'Timing Accel'!$F5*1000000</f>
-        <v>5.8519995550593462</v>
+        <f>'Timing CPU'!C5/'Timing Accel'!$G5*1000000</f>
+        <v>7.0758746771409573</v>
       </c>
       <c r="D6" s="25">
-        <f>'Timing CPU'!D5/'Timing Accel'!$F5*1000000</f>
-        <v>6.83086899381615</v>
+        <f>'Timing CPU'!D5/'Timing Accel'!$G5*1000000</f>
+        <v>8.2594628522183573</v>
       </c>
       <c r="E6" s="23">
         <f>'Timing CPU'!E5/'Timing Accel'!$G5*1000000</f>
@@ -2700,16 +2697,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="23">
-        <f>'Timing CPU'!B6/'Timing Accel'!$F6*1000000</f>
-        <v>87.395232883509394</v>
+        <f>'Timing CPU'!B6/'Timing Accel'!$G6*1000000</f>
+        <v>114.30571940664235</v>
       </c>
       <c r="C7" s="24">
-        <f>'Timing CPU'!C6/'Timing Accel'!$F6*1000000</f>
-        <v>3.5644512846858971</v>
+        <f>'Timing CPU'!C6/'Timing Accel'!$G6*1000000</f>
+        <v>4.6620067816402759</v>
       </c>
       <c r="D7" s="25">
-        <f>'Timing CPU'!D6/'Timing Accel'!$F6*1000000</f>
-        <v>6.5872330210948515</v>
+        <f>'Timing CPU'!D6/'Timing Accel'!$G6*1000000</f>
+        <v>8.6155546994086993</v>
       </c>
       <c r="E7" s="23">
         <f>'Timing CPU'!E6/'Timing Accel'!$G6*1000000</f>
@@ -2750,16 +2747,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="23">
-        <f>'Timing CPU'!B8/'Timing Accel'!$F8*1000000</f>
-        <v>111.76533443886237</v>
+        <f>'Timing CPU'!B8/'Timing Accel'!$G8*1000000</f>
+        <v>166.55768782962463</v>
       </c>
       <c r="C9" s="24">
-        <f>'Timing CPU'!C8/'Timing Accel'!$F8*1000000</f>
-        <v>5.0354233641916268</v>
+        <f>'Timing CPU'!C8/'Timing Accel'!$G8*1000000</f>
+        <v>7.5040125544634284</v>
       </c>
       <c r="D9" s="25">
-        <f>'Timing CPU'!D8/'Timing Accel'!$F8*1000000</f>
-        <v>8.9511446730571258</v>
+        <f>'Timing CPU'!D8/'Timing Accel'!$G8*1000000</f>
+        <v>13.339395150187599</v>
       </c>
       <c r="E9" s="23">
         <f>'Timing CPU'!E8/'Timing Accel'!$G8*1000000</f>
@@ -2787,16 +2784,16 @@
         <v>0</v>
       </c>
       <c r="B10" s="23">
-        <f>'Timing CPU'!B9/'Timing Accel'!$F9*1000000</f>
-        <v>134.00590889125701</v>
+        <f>'Timing CPU'!B9/'Timing Accel'!$G9*1000000</f>
+        <v>198.21957959594749</v>
       </c>
       <c r="C10" s="24">
-        <f>'Timing CPU'!C9/'Timing Accel'!$F9*1000000</f>
-        <v>7.1065783369826887</v>
+        <f>'Timing CPU'!C9/'Timing Accel'!$G9*1000000</f>
+        <v>10.511946689346935</v>
       </c>
       <c r="D10" s="25">
-        <f>'Timing CPU'!D9/'Timing Accel'!$F9*1000000</f>
-        <v>9.7685731197491155</v>
+        <f>'Timing CPU'!D9/'Timing Accel'!$G9*1000000</f>
+        <v>14.449530420484875</v>
       </c>
       <c r="E10" s="23">
         <f>'Timing CPU'!E9/'Timing Accel'!$G9*1000000</f>

</xml_diff>

<commit_message>
Added ZYNQ results to Excel
</commit_message>
<xml_diff>
--- a/sim/knn_datasets.xlsx
+++ b/sim/knn_datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaovieira/Documents/[DOCUMENTS].academic/[2018-now].inesc-id/KNNSimulator/sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1873D2B-8C54-4641-9E1F-BF2BF534878A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE03B50-A7C0-EE4F-8DCD-9CD363DA3DE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" activeTab="2" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" activeTab="6" xr2:uid="{14763823-760A-3243-A6EA-35D5E21ABEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
   <si>
     <t>Poker Hand</t>
   </si>
@@ -201,21 +201,6 @@
     <t>Intel(R) Xeon(R) CPU E5450 @ 3.00GHz (x2)</t>
   </si>
   <si>
-    <t>Cache</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>Capacity</t>
-  </si>
-  <si>
-    <t>Associativity</t>
-  </si>
-  <si>
-    <t>Separate data/instruction</t>
-  </si>
-  <si>
     <t>Designation</t>
   </si>
   <si>
@@ -241,6 +226,9 @@
   </si>
   <si>
     <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>ZYNQ</t>
   </si>
 </sst>
 </file>
@@ -678,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,20 +743,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -787,30 +764,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -838,12 +794,85 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1314,7 +1343,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1529,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC5BBDF-4529-454A-B47D-B01993F61E5D}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1543,93 +1572,70 @@
     <col min="4" max="4" width="11" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="42" customFormat="1">
-      <c r="A1" s="33"/>
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="1:9" s="87" customFormat="1">
+      <c r="A1" s="80"/>
+      <c r="B1" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44" t="s">
+      <c r="C1" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="86"/>
+    </row>
+    <row r="2" spans="1:9" s="37" customFormat="1" ht="17" thickBot="1">
+      <c r="A2" s="81"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="51"/>
-    </row>
-    <row r="2" spans="1:12" s="42" customFormat="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="64" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="65"/>
-    </row>
-    <row r="3" spans="1:12" s="44" customFormat="1" ht="17" thickBot="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="44" t="s">
+      <c r="E2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="H2" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="I2" s="39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="34" customFormat="1">
+    <row r="3" spans="1:9" s="78" customFormat="1" ht="17" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="79"/>
+    </row>
+    <row r="4" spans="1:9" s="34" customFormat="1">
       <c r="A4" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="44">
         <v>3.9</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="44" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="34">
@@ -1641,12 +1647,12 @@
       <c r="G4" s="40">
         <v>1</v>
       </c>
-      <c r="K4" s="47">
+      <c r="H4" s="44">
         <v>0.5</v>
       </c>
-      <c r="L4" s="40"/>
-    </row>
-    <row r="5" spans="1:12" s="15" customFormat="1">
+      <c r="I4" s="40"/>
+    </row>
+    <row r="5" spans="1:9" s="15" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1665,19 +1671,19 @@
       <c r="G5" s="16">
         <v>4</v>
       </c>
-      <c r="K5" s="48">
+      <c r="H5" s="45">
         <v>2</v>
       </c>
-      <c r="L5" s="16"/>
-    </row>
-    <row r="6" spans="1:12" s="36" customFormat="1" ht="17" thickBot="1">
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" s="36" customFormat="1" ht="17" thickBot="1">
       <c r="A6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="46">
         <v>4.7</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="46" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="36">
@@ -1689,18 +1695,18 @@
       <c r="G6" s="41">
         <v>4</v>
       </c>
-      <c r="K6" s="49">
+      <c r="H6" s="46">
         <v>1</v>
       </c>
-      <c r="L6" s="41">
+      <c r="I6" s="41">
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="45">
         <v>145</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -1715,18 +1721,18 @@
       <c r="G7" s="16">
         <v>4</v>
       </c>
-      <c r="K7" s="48">
+      <c r="H7" s="45">
         <v>4</v>
       </c>
-      <c r="L7" s="16">
+      <c r="I7" s="16">
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="45">
         <v>62</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1741,14 +1747,14 @@
       <c r="G8" s="16">
         <v>8</v>
       </c>
-      <c r="K8" s="48">
+      <c r="H8" s="45">
         <v>16</v>
       </c>
-      <c r="L8" s="16">
+      <c r="I8" s="16">
         <v>2133</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1767,14 +1773,14 @@
       <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="K9" s="48">
+      <c r="H9" s="45">
         <v>8</v>
       </c>
-      <c r="L9" s="16">
+      <c r="I9" s="16">
         <v>1600</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1793,14 +1799,14 @@
       <c r="G10" s="16">
         <v>2</v>
       </c>
-      <c r="K10" s="48">
+      <c r="H10" s="45">
         <v>4</v>
       </c>
-      <c r="L10" s="16">
+      <c r="I10" s="16">
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1811,7 +1817,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E11" s="19">
         <v>3</v>
@@ -1822,19 +1828,19 @@
       <c r="G11" s="16">
         <v>8</v>
       </c>
-      <c r="K11" s="48">
+      <c r="H11" s="45">
         <v>32</v>
       </c>
-      <c r="L11" s="16">
+      <c r="I11" s="16">
         <v>667</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1844,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79F4154-E46F-0B4B-835A-2ED02CD556D0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -2065,14 +2071,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="21" customFormat="1">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2084,302 +2090,331 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA235694-7F53-A442-A1E2-343363CCD256}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="89" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="17" thickBot="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="88">
+        <v>6.8800000000000003E-4</v>
+      </c>
+      <c r="C2" s="14">
         <v>2.6689999999999999E-3</v>
       </c>
-      <c r="C2" s="15">
+      <c r="D2" s="15">
         <v>6.9899999999999997E-4</v>
       </c>
-      <c r="D2" s="16">
+      <c r="E2" s="16">
         <v>1.168E-3</v>
       </c>
-      <c r="E2" s="19">
+      <c r="F2" s="19">
         <v>9.9099999999999991E-4</v>
       </c>
-      <c r="F2" s="19">
+      <c r="G2" s="19">
         <v>2.0100000000000001E-4</v>
       </c>
-      <c r="G2" s="19">
+      <c r="H2" s="19">
         <v>2.1699999999999999E-4</v>
       </c>
-      <c r="H2" s="19">
+      <c r="I2" s="19">
         <v>4.7699999999999999E-4</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>5.3300000000000005E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="88">
+        <v>2.036E-3</v>
+      </c>
+      <c r="C3" s="14">
         <v>4.6080000000000001E-3</v>
       </c>
-      <c r="C3" s="15">
+      <c r="D3" s="15">
         <v>1.108E-3</v>
       </c>
-      <c r="D3" s="16">
+      <c r="E3" s="16">
         <v>1.5679999999999999E-3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1.039E-3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1.92E-4</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3.86E-4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>8.7699999999999996E-4</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5.7700000000000004E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="88">
+        <v>4.1023999999999998E-2</v>
+      </c>
+      <c r="C4" s="14">
         <v>9.5048999999999995E-2</v>
       </c>
-      <c r="C4" s="15">
+      <c r="D4" s="15">
         <v>1.2413E-2</v>
       </c>
-      <c r="D4" s="16">
+      <c r="E4" s="16">
         <v>1.0874999999999999E-2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1.98E-3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6.9300000000000004E-4</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2.5690000000000001E-3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.2605999999999999E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.817E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="88">
+        <v>0.11864</v>
+      </c>
+      <c r="C5" s="14">
         <v>0.28378500000000001</v>
       </c>
-      <c r="C5" s="15">
+      <c r="D5" s="15">
         <v>2.8409E-2</v>
       </c>
-      <c r="D5" s="16">
+      <c r="E5" s="16">
         <v>3.3161000000000003E-2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>4.9870000000000001E-3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1.5629999999999999E-3</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.1422E-2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>3.8371000000000002E-2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>6.0299999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="88">
+        <v>0.90632800000000002</v>
+      </c>
+      <c r="C6" s="14">
         <v>2.3883779999999999</v>
       </c>
-      <c r="C6" s="15">
+      <c r="D6" s="15">
         <v>9.7410999999999998E-2</v>
       </c>
-      <c r="D6" s="16">
+      <c r="E6" s="16">
         <v>0.18001900000000001</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2.6360999999999999E-2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>5.6100000000000004E-3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>5.5782999999999999E-2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.260853</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2.1000999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="88">
+        <v>233.51242400000001</v>
+      </c>
+      <c r="C7" s="14">
         <v>631.32241399999998</v>
       </c>
-      <c r="C7" s="15">
+      <c r="D7" s="15">
         <v>30.971461999999999</v>
       </c>
-      <c r="D7" s="16">
+      <c r="E7" s="16">
         <v>50.295641000000003</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>4.6477719999999998</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2.0323419999999999</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>5.6928530000000004</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>58.159612000000003</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3.7200829999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="88">
+        <v>185.311128</v>
+      </c>
+      <c r="C8" s="14">
         <v>515.10249299999998</v>
       </c>
-      <c r="C8" s="15">
+      <c r="D8" s="15">
         <v>23.207187999999999</v>
       </c>
-      <c r="D8" s="16">
+      <c r="E8" s="16">
         <v>41.253909</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>4.0887440000000002</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1.213212</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>4.0199480000000003</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>47.687243000000002</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.669341</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="88">
+        <v>7336.9691590000002</v>
+      </c>
+      <c r="C9" s="14">
         <v>21582.630055000001</v>
       </c>
-      <c r="C9" s="15">
+      <c r="D9" s="15">
         <v>1144.566329</v>
       </c>
-      <c r="D9" s="16">
+      <c r="E9" s="16">
         <v>1573.300025</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>233.37815399999999</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>55.778759000000001</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>171.73456200000001</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1929.127624</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>94.056090999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="20" customFormat="1">
-      <c r="A10" s="74" t="s">
+    <row r="10" spans="1:10" s="20" customFormat="1">
+      <c r="A10" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2387,247 +2422,260 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93596D3-9253-B144-BE5D-2C514E5B9E89}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="5" style="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="17" thickBot="1">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A1" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="55" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="G2" s="55">
+        <v>79</v>
+      </c>
+      <c r="H2" s="55">
+        <v>15</v>
+      </c>
+      <c r="I2" s="55">
+        <v>45</v>
+      </c>
+      <c r="J2" s="55">
+        <v>74</v>
+      </c>
+      <c r="K2" s="13">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="64"/>
+      <c r="B3" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="G3" s="13">
+        <v>95</v>
+      </c>
+      <c r="H3" s="13">
+        <v>20</v>
+      </c>
+      <c r="I3" s="13">
+        <v>52</v>
+      </c>
+      <c r="J3" s="13">
+        <v>83</v>
+      </c>
+      <c r="K3" s="13">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="64"/>
+      <c r="B4" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="73"/>
+      <c r="G4" s="13">
+        <v>83.400249876800004</v>
+      </c>
+      <c r="H4" s="13">
+        <v>17.063609822899998</v>
+      </c>
+      <c r="I4" s="13">
+        <v>48.795460974400001</v>
+      </c>
+      <c r="J4" s="13">
+        <v>78.114444090500001</v>
+      </c>
+      <c r="K4" s="13">
+        <v>233.106558621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="53" customFormat="1">
+      <c r="A5" s="65"/>
+      <c r="B5" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="60">
+      <c r="C5" s="74"/>
+      <c r="D5" s="52"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="56">
+        <v>2.5453206508499999</v>
+      </c>
+      <c r="H5" s="56">
+        <v>1.03317437585</v>
+      </c>
+      <c r="I5" s="56">
+        <v>1.1970549137399999</v>
+      </c>
+      <c r="J5" s="56">
+        <v>1.9350476632</v>
+      </c>
+      <c r="K5" s="56">
+        <v>4.1344574757599997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="73"/>
+      <c r="G6" s="13">
+        <v>82</v>
+      </c>
+      <c r="H6" s="13">
+        <v>16</v>
+      </c>
+      <c r="I6" s="13">
+        <v>48</v>
+      </c>
+      <c r="J6" s="13">
+        <v>74</v>
+      </c>
+      <c r="K6" s="13">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="64"/>
+      <c r="B7" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="73"/>
+      <c r="G7" s="13">
+        <v>161</v>
+      </c>
+      <c r="H7" s="13">
+        <v>66</v>
+      </c>
+      <c r="I7" s="13">
         <v>79</v>
       </c>
-      <c r="G2" s="60">
-        <v>15</v>
-      </c>
-      <c r="H2" s="60">
-        <v>45</v>
-      </c>
-      <c r="I2" s="60">
-        <v>74</v>
-      </c>
-      <c r="J2" s="13">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="76"/>
-      <c r="B3" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="13">
-        <v>95</v>
-      </c>
-      <c r="G3" s="13">
-        <v>20</v>
-      </c>
-      <c r="H3" s="13">
-        <v>52</v>
-      </c>
-      <c r="I3" s="13">
-        <v>83</v>
-      </c>
-      <c r="J3" s="13">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="76"/>
-      <c r="B4" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="13">
-        <v>83.400249876800004</v>
-      </c>
-      <c r="G4" s="13">
-        <v>17.063609822899998</v>
-      </c>
-      <c r="H4" s="13">
-        <v>48.795460974400001</v>
-      </c>
-      <c r="I4" s="13">
-        <v>78.114444090500001</v>
-      </c>
-      <c r="J4" s="13">
-        <v>233.106558621</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="58" customFormat="1">
-      <c r="A5" s="77"/>
-      <c r="B5" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="57"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="61">
-        <v>2.5453206508499999</v>
-      </c>
-      <c r="G5" s="61">
-        <v>1.03317437585</v>
-      </c>
-      <c r="H5" s="61">
-        <v>1.1970549137399999</v>
-      </c>
-      <c r="I5" s="61">
-        <v>1.9350476632</v>
-      </c>
-      <c r="J5" s="61">
-        <v>4.1344574757599997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="55" t="s">
+      <c r="J7" s="57">
+        <v>149</v>
+      </c>
+      <c r="K7" s="58">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="64"/>
+      <c r="B8" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="73"/>
+      <c r="G8" s="13">
+        <v>150.733263029</v>
+      </c>
+      <c r="H8" s="13">
+        <v>55.030479873300003</v>
+      </c>
+      <c r="I8" s="13">
+        <v>74.802833365300003</v>
+      </c>
+      <c r="J8" s="13">
+        <v>141.69338719699999</v>
+      </c>
+      <c r="K8" s="13">
+        <v>330.97444960000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="64"/>
+      <c r="B9" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="13">
-        <v>82</v>
-      </c>
-      <c r="G6" s="13">
-        <v>16</v>
-      </c>
-      <c r="H6" s="13">
-        <v>48</v>
-      </c>
-      <c r="I6" s="13">
-        <v>74</v>
-      </c>
-      <c r="J6" s="13">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="76"/>
-      <c r="B7" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="13">
-        <v>161</v>
-      </c>
-      <c r="G7" s="13">
-        <v>66</v>
-      </c>
-      <c r="H7" s="13">
-        <v>79</v>
-      </c>
-      <c r="I7" s="62">
-        <v>149</v>
-      </c>
-      <c r="J7" s="63">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="76"/>
-      <c r="B8" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="13">
-        <v>150.733263029</v>
-      </c>
-      <c r="G8" s="13">
-        <v>55.030479873300003</v>
-      </c>
-      <c r="H8" s="13">
-        <v>74.802833365300003</v>
-      </c>
-      <c r="I8" s="13">
-        <v>141.69338719699999</v>
-      </c>
-      <c r="J8" s="13">
-        <v>330.97444960000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="76"/>
-      <c r="B9" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="13">
+      <c r="C9" s="73"/>
+      <c r="G9" s="13">
         <v>0.10434324846</v>
       </c>
-      <c r="G9" s="13">
+      <c r="H9" s="13">
         <v>0.14542360448300001</v>
       </c>
-      <c r="H9" s="13">
+      <c r="I9" s="13">
         <v>8.3724022653700006E-2</v>
       </c>
-      <c r="I9" s="13">
+      <c r="J9" s="13">
         <v>3.1785635094099998E-2</v>
       </c>
-      <c r="J9" s="13">
+      <c r="K9" s="13">
         <v>0.21005931907200001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="20" customFormat="1">
-      <c r="A10" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+    <row r="10" spans="1:11" s="20" customFormat="1">
+      <c r="A10" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A10:K10"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
   </mergeCells>
@@ -2637,344 +2685,386 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40F9C77-6425-6D4E-BBF1-9B74B3972FC3}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" style="72" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="42" customFormat="1">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:10" s="42" customFormat="1">
+      <c r="B1" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="78" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="80"/>
-    </row>
-    <row r="2" spans="1:9" s="43" customFormat="1" ht="17" thickBot="1">
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
+    </row>
+    <row r="2" spans="1:10" s="43" customFormat="1" ht="17" thickBot="1">
       <c r="A2" s="38"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="F2" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="H2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="I2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="J2" s="39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="70">
         <f>'Timing CPU'!B2/'Timing Accel'!$G2*1000000</f>
-        <v>9.106417823876626</v>
+        <v>2.3474018219659496</v>
       </c>
       <c r="C3" s="24">
         <f>'Timing CPU'!C2/'Timing Accel'!$G2*1000000</f>
+        <v>9.106417823876626</v>
+      </c>
+      <c r="D3" s="24">
+        <f>'Timing CPU'!D2/'Timing Accel'!$G2*1000000</f>
         <v>2.3849329557473813</v>
       </c>
-      <c r="D3" s="25">
-        <f>'Timing CPU'!D2/'Timing Accel'!$G2*1000000</f>
+      <c r="E3" s="25">
+        <f>'Timing CPU'!E2/'Timing Accel'!$G2*1000000</f>
         <v>3.9851240233375416</v>
       </c>
-      <c r="E3" s="23">
-        <f>'Timing CPU'!E2/'Timing Accel'!$G2*1000000</f>
+      <c r="F3" s="23">
+        <f>'Timing CPU'!F2/'Timing Accel'!$G2*1000000</f>
         <v>3.3812139615817669</v>
-      </c>
-      <c r="F3" s="24">
-        <f>'Timing CPU'!F2/'Timing Accel'!$G2*1000000</f>
-        <v>0.68579617182435437</v>
       </c>
       <c r="G3" s="24">
         <f>'Timing CPU'!G2/'Timing Accel'!$G2*1000000</f>
-        <v>0.74038691187007399</v>
+        <v>0.68579617182435437</v>
       </c>
       <c r="H3" s="24">
         <f>'Timing CPU'!H2/'Timing Accel'!$G2*1000000</f>
+        <v>0.74038691187007399</v>
+      </c>
+      <c r="I3" s="24">
+        <f>'Timing CPU'!I2/'Timing Accel'!$G2*1000000</f>
         <v>1.62748643761302</v>
       </c>
-      <c r="I3" s="25">
-        <f>'Timing CPU'!I2/'Timing Accel'!$G2*1000000</f>
+      <c r="J3" s="25">
+        <f>'Timing CPU'!J2/'Timing Accel'!$G2*1000000</f>
         <v>1.8185540277730394</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="70">
         <f>'Timing CPU'!B3/'Timing Accel'!$G3*1000000</f>
-        <v>13.85697961147531</v>
+        <v>6.1225717206952543</v>
       </c>
       <c r="C4" s="24">
         <f>'Timing CPU'!C3/'Timing Accel'!$G3*1000000</f>
+        <v>13.85697961147531</v>
+      </c>
+      <c r="D4" s="24">
+        <f>'Timing CPU'!D3/'Timing Accel'!$G3*1000000</f>
         <v>3.3319299933842546</v>
       </c>
-      <c r="D4" s="25">
-        <f>'Timing CPU'!D3/'Timing Accel'!$G3*1000000</f>
+      <c r="E4" s="25">
+        <f>'Timing CPU'!E3/'Timing Accel'!$G3*1000000</f>
         <v>4.7152222289047927</v>
       </c>
-      <c r="E4" s="23">
-        <f>'Timing CPU'!E3/'Timing Accel'!$G3*1000000</f>
+      <c r="F4" s="23">
+        <f>'Timing CPU'!F3/'Timing Accel'!$G3*1000000</f>
         <v>3.1244361580561733</v>
-      </c>
-      <c r="F4" s="24">
-        <f>'Timing CPU'!F3/'Timing Accel'!$G3*1000000</f>
-        <v>0.57737415047813789</v>
       </c>
       <c r="G4" s="24">
         <f>'Timing CPU'!G3/'Timing Accel'!$G3*1000000</f>
-        <v>1.1607626150237564</v>
+        <v>0.57737415047813789</v>
       </c>
       <c r="H4" s="24">
         <f>'Timing CPU'!H3/'Timing Accel'!$G3*1000000</f>
+        <v>1.1607626150237564</v>
+      </c>
+      <c r="I4" s="24">
+        <f>'Timing CPU'!I3/'Timing Accel'!$G3*1000000</f>
         <v>2.6372767185902446</v>
       </c>
-      <c r="I4" s="25">
-        <f>'Timing CPU'!I3/'Timing Accel'!$G3*1000000</f>
+      <c r="J4" s="25">
+        <f>'Timing CPU'!J3/'Timing Accel'!$G3*1000000</f>
         <v>1.7351296084681542</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="70">
         <f>'Timing CPU'!B4/'Timing Accel'!$G4*1000000</f>
-        <v>56.67461689821716</v>
+        <v>24.461272434559657</v>
       </c>
       <c r="C5" s="24">
         <f>'Timing CPU'!C4/'Timing Accel'!$G4*1000000</f>
+        <v>56.67461689821716</v>
+      </c>
+      <c r="D5" s="24">
+        <f>'Timing CPU'!D4/'Timing Accel'!$G4*1000000</f>
         <v>7.401466817721067</v>
       </c>
-      <c r="D5" s="25">
-        <f>'Timing CPU'!D4/'Timing Accel'!$G4*1000000</f>
+      <c r="E5" s="25">
+        <f>'Timing CPU'!E4/'Timing Accel'!$G4*1000000</f>
         <v>6.484407608371594</v>
       </c>
-      <c r="E5" s="23">
-        <f>'Timing CPU'!E4/'Timing Accel'!$G4*1000000</f>
+      <c r="F5" s="23">
+        <f>'Timing CPU'!F4/'Timing Accel'!$G4*1000000</f>
         <v>1.1806093852483455</v>
-      </c>
-      <c r="F5" s="24">
-        <f>'Timing CPU'!F4/'Timing Accel'!$G4*1000000</f>
-        <v>0.41321328483692094</v>
       </c>
       <c r="G5" s="24">
         <f>'Timing CPU'!G4/'Timing Accel'!$G4*1000000</f>
-        <v>1.5318108639914139</v>
+        <v>0.41321328483692094</v>
       </c>
       <c r="H5" s="24">
         <f>'Timing CPU'!H4/'Timing Accel'!$G4*1000000</f>
+        <v>1.5318108639914139</v>
+      </c>
+      <c r="I5" s="24">
+        <f>'Timing CPU'!I4/'Timing Accel'!$G4*1000000</f>
         <v>7.5165464194144649</v>
       </c>
-      <c r="I5" s="25">
-        <f>'Timing CPU'!I4/'Timing Accel'!$G4*1000000</f>
+      <c r="J5" s="25">
+        <f>'Timing CPU'!J4/'Timing Accel'!$G4*1000000</f>
         <v>1.0834178045435574</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="70">
         <f>'Timing CPU'!B5/'Timing Accel'!$G5*1000000</f>
-        <v>70.682779937781916</v>
+        <v>29.549852923228666</v>
       </c>
       <c r="C6" s="24">
         <f>'Timing CPU'!C5/'Timing Accel'!$G5*1000000</f>
+        <v>70.682779937781916</v>
+      </c>
+      <c r="D6" s="24">
+        <f>'Timing CPU'!D5/'Timing Accel'!$G5*1000000</f>
         <v>7.0758746771409573</v>
       </c>
-      <c r="D6" s="25">
-        <f>'Timing CPU'!D5/'Timing Accel'!$G5*1000000</f>
+      <c r="E6" s="25">
+        <f>'Timing CPU'!E5/'Timing Accel'!$G5*1000000</f>
         <v>8.2594628522183573</v>
       </c>
-      <c r="E6" s="23">
-        <f>'Timing CPU'!E5/'Timing Accel'!$G5*1000000</f>
+      <c r="F6" s="23">
+        <f>'Timing CPU'!F5/'Timing Accel'!$G5*1000000</f>
         <v>1.2421199977085415</v>
-      </c>
-      <c r="F6" s="24">
-        <f>'Timing CPU'!F5/'Timing Accel'!$G5*1000000</f>
-        <v>0.38929888839351318</v>
       </c>
       <c r="G6" s="24">
         <f>'Timing CPU'!G5/'Timing Accel'!$G5*1000000</f>
-        <v>2.8448956514591859</v>
+        <v>0.38929888839351318</v>
       </c>
       <c r="H6" s="24">
         <f>'Timing CPU'!H5/'Timing Accel'!$G5*1000000</f>
+        <v>2.8448956514591859</v>
+      </c>
+      <c r="I6" s="24">
+        <f>'Timing CPU'!I5/'Timing Accel'!$G5*1000000</f>
         <v>9.5571258135300674</v>
       </c>
-      <c r="I6" s="25">
-        <f>'Timing CPU'!I5/'Timing Accel'!$G5*1000000</f>
+      <c r="J6" s="25">
+        <f>'Timing CPU'!J5/'Timing Accel'!$G5*1000000</f>
         <v>1.5019016615565481</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="70">
         <f>'Timing CPU'!B6/'Timing Accel'!$G6*1000000</f>
-        <v>114.30571940664235</v>
+        <v>43.37607952274864</v>
       </c>
       <c r="C7" s="24">
         <f>'Timing CPU'!C6/'Timing Accel'!$G6*1000000</f>
+        <v>114.30571940664235</v>
+      </c>
+      <c r="D7" s="24">
+        <f>'Timing CPU'!D6/'Timing Accel'!$G6*1000000</f>
         <v>4.6620067816402759</v>
       </c>
-      <c r="D7" s="25">
-        <f>'Timing CPU'!D6/'Timing Accel'!$G6*1000000</f>
+      <c r="E7" s="25">
+        <f>'Timing CPU'!E6/'Timing Accel'!$G6*1000000</f>
         <v>8.6155546994086993</v>
       </c>
-      <c r="E7" s="23">
-        <f>'Timing CPU'!E6/'Timing Accel'!$G6*1000000</f>
+      <c r="F7" s="23">
+        <f>'Timing CPU'!F6/'Timing Accel'!$G6*1000000</f>
         <v>1.2616148152756803</v>
-      </c>
-      <c r="F7" s="24">
-        <f>'Timing CPU'!F6/'Timing Accel'!$G6*1000000</f>
-        <v>0.26848978087692305</v>
       </c>
       <c r="G7" s="24">
         <f>'Timing CPU'!G6/'Timing Accel'!$G6*1000000</f>
-        <v>2.6697264610797502</v>
+        <v>0.26848978087692305</v>
       </c>
       <c r="H7" s="24">
         <f>'Timing CPU'!H6/'Timing Accel'!$G6*1000000</f>
+        <v>2.6697264610797502</v>
+      </c>
+      <c r="I7" s="24">
+        <f>'Timing CPU'!I6/'Timing Accel'!$G6*1000000</f>
         <v>12.484200501085205</v>
       </c>
-      <c r="I7" s="25">
-        <f>'Timing CPU'!I6/'Timing Accel'!$G6*1000000</f>
+      <c r="J7" s="25">
+        <f>'Timing CPU'!J6/'Timing Accel'!$G6*1000000</f>
         <v>1.0050898196428271</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="30" customFormat="1">
+    <row r="8" spans="1:10" s="30" customFormat="1">
       <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="29"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="70">
         <f>'Timing CPU'!B8/'Timing Accel'!$G8*1000000</f>
-        <v>166.55768782962463</v>
+        <v>59.920100229022985</v>
       </c>
       <c r="C9" s="24">
         <f>'Timing CPU'!C8/'Timing Accel'!$G8*1000000</f>
+        <v>166.55768782962463</v>
+      </c>
+      <c r="D9" s="24">
+        <f>'Timing CPU'!D8/'Timing Accel'!$G8*1000000</f>
         <v>7.5040125544634284</v>
       </c>
-      <c r="D9" s="25">
-        <f>'Timing CPU'!D8/'Timing Accel'!$G8*1000000</f>
+      <c r="E9" s="25">
+        <f>'Timing CPU'!E8/'Timing Accel'!$G8*1000000</f>
         <v>13.339395150187599</v>
       </c>
-      <c r="E9" s="23">
-        <f>'Timing CPU'!E8/'Timing Accel'!$G8*1000000</f>
+      <c r="F9" s="23">
+        <f>'Timing CPU'!F8/'Timing Accel'!$G8*1000000</f>
         <v>1.3220897899386612</v>
-      </c>
-      <c r="F9" s="24">
-        <f>'Timing CPU'!F8/'Timing Accel'!$G8*1000000</f>
-        <v>0.39229044377223493</v>
       </c>
       <c r="G9" s="24">
         <f>'Timing CPU'!G8/'Timing Accel'!$G8*1000000</f>
-        <v>1.2998446972675086</v>
+        <v>0.39229044377223493</v>
       </c>
       <c r="H9" s="24">
         <f>'Timing CPU'!H8/'Timing Accel'!$G8*1000000</f>
+        <v>1.2998446972675086</v>
+      </c>
+      <c r="I9" s="24">
+        <f>'Timing CPU'!I8/'Timing Accel'!$G8*1000000</f>
         <v>15.419604915500676</v>
       </c>
-      <c r="I9" s="25">
-        <f>'Timing CPU'!I8/'Timing Accel'!$G8*1000000</f>
+      <c r="J9" s="25">
+        <f>'Timing CPU'!J8/'Timing Accel'!$G8*1000000</f>
         <v>0.53977913315824977</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="70">
         <f>'Timing CPU'!B9/'Timing Accel'!$G9*1000000</f>
-        <v>198.21957959594749</v>
+        <v>67.384324269066113</v>
       </c>
       <c r="C10" s="24">
         <f>'Timing CPU'!C9/'Timing Accel'!$G9*1000000</f>
+        <v>198.21957959594749</v>
+      </c>
+      <c r="D10" s="24">
+        <f>'Timing CPU'!D9/'Timing Accel'!$G9*1000000</f>
         <v>10.511946689346935</v>
       </c>
-      <c r="D10" s="25">
-        <f>'Timing CPU'!D9/'Timing Accel'!$G9*1000000</f>
+      <c r="E10" s="25">
+        <f>'Timing CPU'!E9/'Timing Accel'!$G9*1000000</f>
         <v>14.449530420484875</v>
       </c>
-      <c r="E10" s="23">
-        <f>'Timing CPU'!E9/'Timing Accel'!$G9*1000000</f>
+      <c r="F10" s="23">
+        <f>'Timing CPU'!F9/'Timing Accel'!$G9*1000000</f>
         <v>2.1433958444763919</v>
-      </c>
-      <c r="F10" s="24">
-        <f>'Timing CPU'!F9/'Timing Accel'!$G9*1000000</f>
-        <v>0.51228428283244609</v>
       </c>
       <c r="G10" s="24">
         <f>'Timing CPU'!G9/'Timing Accel'!$G9*1000000</f>
-        <v>1.57724765679556</v>
+        <v>0.51228428283244609</v>
       </c>
       <c r="H10" s="24">
         <f>'Timing CPU'!H9/'Timing Accel'!$G9*1000000</f>
+        <v>1.57724765679556</v>
+      </c>
+      <c r="I10" s="24">
+        <f>'Timing CPU'!I9/'Timing Accel'!$G9*1000000</f>
         <v>17.717528662713718</v>
       </c>
-      <c r="I10" s="25">
-        <f>'Timing CPU'!I9/'Timing Accel'!$G9*1000000</f>
+      <c r="J10" s="25">
+        <f>'Timing CPU'!J9/'Timing Accel'!$G9*1000000</f>
         <v>0.86383164465810869</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:I7 B9:I10">
+  <conditionalFormatting sqref="B3:B7 B9:B10 D9:J10 D3:J7">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C7 C9:C10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>